<commit_message>
Energy added to the score
</commit_message>
<xml_diff>
--- a/data/RDI.xlsx
+++ b/data/RDI.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t xml:space="preserve">nutrient</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t xml:space="preserve">Biotin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calories</t>
   </si>
   <si>
     <t xml:space="preserve">Calcium</t>
@@ -333,10 +336,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C40" activeCellId="0" sqref="C40"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -380,15 +383,15 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="n">
-        <v>1000</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>1000</v>
+      <c r="B4" s="0" t="n">
+        <v>2400</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>2000</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -396,10 +399,10 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>130000</v>
+        <v>1000</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>130000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -407,10 +410,10 @@
         <v>7</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>2300</v>
+        <v>130000</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>2300</v>
+        <v>130000</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -418,21 +421,21 @@
         <v>8</v>
       </c>
       <c r="B7" s="1" t="n">
-        <v>550</v>
+        <v>2300</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>425</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="0" t="n">
-        <v>0.035</v>
-      </c>
-      <c r="C8" s="0" t="n">
-        <v>0.025</v>
+      <c r="B8" s="1" t="n">
+        <v>550</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>425</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -440,21 +443,21 @@
         <v>10</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>0.9</v>
+        <v>0.035</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>0.9</v>
+        <v>0.025</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="1" t="n">
-        <v>65000</v>
-      </c>
-      <c r="C10" s="1" t="n">
-        <v>65000</v>
+      <c r="B10" s="0" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>0.9</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -462,21 +465,21 @@
         <v>12</v>
       </c>
       <c r="B11" s="1" t="n">
-        <v>38000</v>
+        <v>65000</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>25000</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="C12" s="0" t="n">
-        <v>3</v>
+      <c r="B12" s="1" t="n">
+        <v>38000</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>25000</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -484,32 +487,32 @@
         <v>14</v>
       </c>
       <c r="B13" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="0" t="n">
         <v>0.4</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="C14" s="0" t="n">
         <v>0.4</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="0" t="n">
+    <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="0" t="n">
         <v>0.15</v>
       </c>
-      <c r="C14" s="0" t="n">
+      <c r="C15" s="0" t="n">
         <v>0.15</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="C15" s="0" t="n">
-        <v>18</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -517,10 +520,10 @@
         <v>17</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>17000</v>
+        <v>8</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>12000</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -528,10 +531,10 @@
         <v>18</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>400</v>
+        <v>17000</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>310</v>
+        <v>12000</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -539,10 +542,10 @@
         <v>19</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>2.3</v>
+        <v>400</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>1.8</v>
+        <v>310</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -550,10 +553,10 @@
         <v>20</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>0.045</v>
+        <v>2.3</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>0.045</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -561,10 +564,10 @@
         <v>21</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>24000</v>
+        <v>0.045</v>
       </c>
       <c r="C20" s="0" t="n">
-        <v>24000</v>
+        <v>0.045</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -572,10 +575,10 @@
         <v>22</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>16</v>
+        <v>24000</v>
       </c>
       <c r="C21" s="0" t="n">
-        <v>14</v>
+        <v>24000</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -583,10 +586,10 @@
         <v>23</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C22" s="0" t="n">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -594,10 +597,10 @@
         <v>24</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>700</v>
+        <v>5</v>
       </c>
       <c r="C23" s="0" t="n">
-        <v>700</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -605,10 +608,10 @@
         <v>25</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>16000</v>
+        <v>700</v>
       </c>
       <c r="C24" s="0" t="n">
-        <v>16000</v>
+        <v>700</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -616,10 +619,10 @@
         <v>26</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>4700</v>
+        <v>16000</v>
       </c>
       <c r="C25" s="0" t="n">
-        <v>4700</v>
+        <v>16000</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -627,21 +630,21 @@
         <v>27</v>
       </c>
       <c r="B26" s="0" t="n">
-        <v>56000</v>
+        <v>4700</v>
       </c>
       <c r="C26" s="0" t="n">
-        <v>46000</v>
+        <v>4700</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="1" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="C27" s="1" t="n">
-        <v>1.1</v>
+      <c r="B27" s="0" t="n">
+        <v>56000</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>46000</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -649,21 +652,21 @@
         <v>29</v>
       </c>
       <c r="B28" s="1" t="n">
-        <v>12000</v>
+        <v>1.3</v>
       </c>
       <c r="C28" s="1" t="n">
-        <v>12000</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="B29" s="0" t="n">
-        <v>0.055</v>
-      </c>
-      <c r="C29" s="0" t="n">
-        <v>0.055</v>
+      <c r="B29" s="1" t="n">
+        <v>12000</v>
+      </c>
+      <c r="C29" s="1" t="n">
+        <v>12000</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -671,10 +674,10 @@
         <v>31</v>
       </c>
       <c r="B30" s="0" t="n">
-        <v>1500</v>
+        <v>0.055</v>
       </c>
       <c r="C30" s="0" t="n">
-        <v>1500</v>
+        <v>0.055</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -682,10 +685,10 @@
         <v>32</v>
       </c>
       <c r="B31" s="0" t="n">
-        <v>39000</v>
+        <v>1500</v>
       </c>
       <c r="C31" s="0" t="n">
-        <v>25000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -693,10 +696,10 @@
         <v>33</v>
       </c>
       <c r="B32" s="0" t="n">
-        <v>1.2</v>
+        <v>39000</v>
       </c>
       <c r="C32" s="0" t="n">
-        <v>1.1</v>
+        <v>25000</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -704,10 +707,10 @@
         <v>34</v>
       </c>
       <c r="B33" s="0" t="n">
-        <v>0.9</v>
+        <v>1.2</v>
       </c>
       <c r="C33" s="0" t="n">
-        <v>0.7</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -715,10 +718,10 @@
         <v>35</v>
       </c>
       <c r="B34" s="0" t="n">
-        <v>1.3</v>
+        <v>0.9</v>
       </c>
       <c r="C34" s="0" t="n">
-        <v>1.3</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -726,10 +729,10 @@
         <v>36</v>
       </c>
       <c r="B35" s="0" t="n">
-        <v>0.0024</v>
+        <v>1.3</v>
       </c>
       <c r="C35" s="0" t="n">
-        <v>0.0024</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -737,10 +740,10 @@
         <v>37</v>
       </c>
       <c r="B36" s="0" t="n">
-        <v>90</v>
+        <v>0.0024</v>
       </c>
       <c r="C36" s="0" t="n">
-        <v>75</v>
+        <v>0.0024</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -748,10 +751,10 @@
         <v>38</v>
       </c>
       <c r="B37" s="0" t="n">
-        <v>0.015</v>
+        <v>90</v>
       </c>
       <c r="C37" s="0" t="n">
-        <v>0.015</v>
+        <v>75</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -759,10 +762,10 @@
         <v>39</v>
       </c>
       <c r="B38" s="0" t="n">
-        <v>15</v>
+        <v>0.015</v>
       </c>
       <c r="C38" s="0" t="n">
-        <v>15</v>
+        <v>0.015</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -770,10 +773,10 @@
         <v>40</v>
       </c>
       <c r="B39" s="0" t="n">
-        <v>0.12</v>
+        <v>15</v>
       </c>
       <c r="C39" s="0" t="n">
-        <v>0.09</v>
+        <v>15</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -781,10 +784,10 @@
         <v>41</v>
       </c>
       <c r="B40" s="0" t="n">
-        <v>3700000</v>
+        <v>0.12</v>
       </c>
       <c r="C40" s="0" t="n">
-        <v>2700000</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -792,9 +795,20 @@
         <v>42</v>
       </c>
       <c r="B41" s="0" t="n">
+        <v>3700000</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>2700000</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B42" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="C41" s="0" t="n">
+      <c r="C42" s="0" t="n">
         <v>8</v>
       </c>
     </row>

</xml_diff>